<commit_message>
se actualizó la doc
</commit_message>
<xml_diff>
--- a/Quiz/Querys/Proyecto Quiz.xlsx
+++ b/Quiz/Querys/Proyecto Quiz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elias\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403634D9-D0D9-450C-8CFB-2A4A9570017E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD49CA08-B013-41BF-88D7-5846D394E2F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="50">
   <si>
     <t>Requerimiento</t>
   </si>
@@ -160,13 +160,28 @@
   </si>
   <si>
     <t>Base de datos que guardará todo lo relacionado con la aplicación</t>
+  </si>
+  <si>
+    <t>Interfaz para mostrar las preguntas</t>
+  </si>
+  <si>
+    <t>Interfaz que mostrará una por una cada pregunta del quiz y sus respectivas opciones</t>
+  </si>
+  <si>
+    <t>Hecho</t>
+  </si>
+  <si>
+    <t>Servicios de inicio de Sesión</t>
+  </si>
+  <si>
+    <t>Servicios que se encargan de iniciar sesión, registrar un usuario o cerrar sesión</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +191,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -314,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -322,9 +345,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -346,11 +366,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="16">
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -377,6 +420,101 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -401,13 +539,12 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
+        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -473,94 +610,26 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -581,6 +650,22 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -596,7 +681,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{57741142-3410-4BC4-AE03-EA9492A1FFFB}" name="Tabla1" displayName="Tabla1" ref="A1:C8" totalsRowShown="0" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{57741142-3410-4BC4-AE03-EA9492A1FFFB}" name="Tabla1" displayName="Tabla1" ref="A1:C8" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12">
   <autoFilter ref="A1:C8" xr:uid="{57741142-3410-4BC4-AE03-EA9492A1FFFB}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{F80572D7-E824-4983-A3AD-33DF9CC8732A}" name="Requerimiento" dataDxfId="11"/>
@@ -608,12 +693,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8FE0BDB4-08DD-4F3D-AA7F-0EECB534E5F9}" name="Tabla2" displayName="Tabla2" ref="A12:E21" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
-  <autoFilter ref="A12:E21" xr:uid="{8FE0BDB4-08DD-4F3D-AA7F-0EECB534E5F9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8FE0BDB4-08DD-4F3D-AA7F-0EECB534E5F9}" name="Tabla2" displayName="Tabla2" ref="A12:E23" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+  <autoFilter ref="A12:E23" xr:uid="{8FE0BDB4-08DD-4F3D-AA7F-0EECB534E5F9}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{9ACC6B09-2A5E-446B-A413-56EC10A3E7FB}" name="Funcion" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{E286E823-E520-45EB-AF17-2D51BBD8A770}" name="Descripción" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{CE63612B-06D0-42E8-8D19-DFBD799FC83A}" name="Requerimiento" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{9ACC6B09-2A5E-446B-A413-56EC10A3E7FB}" name="Funcion" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{E286E823-E520-45EB-AF17-2D51BBD8A770}" name="Descripción" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{CE63612B-06D0-42E8-8D19-DFBD799FC83A}" name="Requerimiento" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{78ECA7F6-6259-4010-A03F-05D719EC7827}" name="Status" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{A13ACD19-7695-47CD-B758-038D8912AF83}" name="Asignado" dataDxfId="0"/>
   </tableColumns>
@@ -884,15 +969,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.28515625" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
@@ -902,113 +987,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="18" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="18" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="18" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="18" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="18" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="18" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="19" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1020,12 +1105,12 @@
       <c r="D13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1037,12 +1122,12 @@
       <c r="D14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1054,12 +1139,12 @@
       <c r="D15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -1071,12 +1156,12 @@
       <c r="D16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -1085,15 +1170,15 @@
       <c r="C17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="13" t="s">
+      <c r="D17" s="20">
+        <v>0.66</v>
+      </c>
+      <c r="E17" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -1103,14 +1188,14 @@
         <v>3</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="21" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -1119,15 +1204,15 @@
       <c r="C19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="13" t="s">
+      <c r="D19" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="22" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -1139,24 +1224,58 @@
       <c r="D20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="12" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" s="14" t="s">
+      <c r="D21" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="13" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>